<commit_message>
- Layout.pptx com estilo de menus - divisaoTarefas.xlsx - 2 itens extra
</commit_message>
<xml_diff>
--- a/Documents/DivisaoTarefas.xlsx
+++ b/Documents/DivisaoTarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>Task</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>Actualizar a lista de atividades sempre que há alterações nos dados</t>
+  </si>
+  <si>
+    <t>Extra:</t>
+  </si>
+  <si>
+    <t>Stuff</t>
+  </si>
+  <si>
+    <t>Opção de Alterar Língua (Inglês, Português, Francês, etc)</t>
+  </si>
+  <si>
+    <t>Opção de Alterar Cores (Neon70s, Hospital Pastels, Dark, Color Blind, White, etc)</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +183,12 @@
         <bgColor rgb="FFD9D2E9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD7E6B"/>
+        <bgColor rgb="FFDD7E6B"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -192,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -212,6 +230,13 @@
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -786,8 +811,27 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="C26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="E27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="9"/>
+    </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1"/>
     <row r="30" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
- colunas no homepage.html
</commit_message>
<xml_diff>
--- a/Documents/DivisaoTarefas.xlsx
+++ b/Documents/DivisaoTarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Grupo de 3 alunos</t>
+  </si>
+  <si>
+    <t>retrospective.html</t>
   </si>
   <si>
     <t>Incluir campos de input para preencher os detalhes do momento de retrospetiva (data, menbros presentes, coméntários)</t>
@@ -153,7 +156,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,18 +166,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -268,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -282,35 +279,32 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -631,16 +625,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="116.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="41.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="116.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="41.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -649,7 +643,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -658,7 +652,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -676,7 +670,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="3" t="s">
@@ -700,19 +694,19 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -721,19 +715,19 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -742,19 +736,19 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="2">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -763,19 +757,19 @@
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>4</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -784,46 +778,48 @@
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5">
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2">
         <v>6</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -831,122 +827,122 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="5">
+      <c r="C13" s="2">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="5">
+      <c r="C14" s="2">
         <v>2</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="9" t="s">
+      <c r="E14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="5">
+      <c r="C15" s="2">
         <v>3</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="D15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="E15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="5">
+      <c r="C16" s="2">
         <v>4</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="9" t="s">
+      <c r="E16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="5">
+      <c r="C17" s="2">
         <v>5</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="9" t="s">
+      <c r="E17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="5">
+      <c r="C18" s="2">
         <v>6</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="9" t="s">
+      <c r="E18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -954,46 +950,46 @@
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="5">
+      <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="5">
+      <c r="C21" s="2">
         <v>2</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="E21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -1001,38 +997,38 @@
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="5">
+      <c r="C23" s="2">
         <v>1</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="F23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="5">
+      <c r="C24" s="2">
         <v>2</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="11" t="s">
+      <c r="E24" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1048,30 +1044,30 @@
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="8" t="s">
-        <v>35</v>
+      <c r="C26" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F26" s="12" t="s">
+      <c r="E26" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="12"/>
+      <c r="F26" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="12" t="s">
+      <c r="E27" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="12"/>
+      <c r="F27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
@@ -1079,10 +1075,10 @@
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1092,10 +1088,10 @@
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G29" s="1"/>
     </row>

</xml_diff>

<commit_message>
- small edits no divisaotarefas.xlsx
</commit_message>
<xml_diff>
--- a/Documents/DivisaoTarefas.xlsx
+++ b/Documents/DivisaoTarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -103,7 +103,7 @@
     <t>Actualizar o nome do utilizador visível no cabeçalho</t>
   </si>
   <si>
-    <t>Submissão do forumlário de retrospetiva com todos os campos atrvés de um botão em Javascript</t>
+    <t>Submissão do formulário de retrospetiva com todos os campos atrvés de um botão em Javascript</t>
   </si>
   <si>
     <t>Persistência - Frontend</t>
@@ -130,25 +130,22 @@
     <t>Stuff 1</t>
   </si>
   <si>
-    <t>Opção de Alterar Língua (Inglês, Português, Francês, etc)</t>
+    <t>Opção de Alterar Língua (Inglês, Português)</t>
   </si>
   <si>
     <t>Stuff 2</t>
   </si>
   <si>
-    <t>Opção de Alterar Cores (Neon70s, Hospital Pastels, Dark, Color Blind, White, etc)</t>
+    <t>Opção de Alterar Cores (Dark, Light)</t>
   </si>
   <si>
     <t>Stuff 3</t>
   </si>
   <si>
-    <t>Opção de Salvar Sugestão de Username</t>
+    <t>Estrela nos favoritos</t>
   </si>
   <si>
-    <t>Stuff 4</t>
-  </si>
-  <si>
-    <t>Ordenar Tasks por favoritos, ou por data</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -265,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -299,6 +296,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -625,13 +625,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="116.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="41.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="116.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="41.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1032,7 +1032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
@@ -1082,20 +1082,20 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>44</v>
+      <c r="F29" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
@@ -1104,7 +1104,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
@@ -1113,7 +1113,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
@@ -1122,7 +1122,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
@@ -1131,7 +1131,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>

</xml_diff>

<commit_message>
- update da DivisaoTarefas e versão no index.html
</commit_message>
<xml_diff>
--- a/Documents/DivisaoTarefas.xlsx
+++ b/Documents/DivisaoTarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -137,12 +137,6 @@
   </si>
   <si>
     <t>Opção de Alterar Cores (Dark, Light)</t>
-  </si>
-  <si>
-    <t>Stuff 3</t>
-  </si>
-  <si>
-    <t>Estrela nos favoritos</t>
   </si>
   <si>
     <t/>
@@ -1074,11 +1068,11 @@
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>42</v>
+      <c r="F28" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1087,12 +1081,8 @@
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>43</v>
-      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
- more edits on DivisaoTarefas
</commit_message>
<xml_diff>
--- a/Documents/DivisaoTarefas.xlsx
+++ b/Documents/DivisaoTarefas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -67,9 +67,6 @@
     <t>homepage.html</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Incluir menu no header para aceder à página de Retrospetiva</t>
   </si>
   <si>
@@ -103,7 +100,7 @@
     <t>Actualizar o nome do utilizador visível no cabeçalho</t>
   </si>
   <si>
-    <t>Submissão do formulário de retrospetiva com todos os campos atrvés de um botão em Javascript</t>
+    <t>Submissão do formulário de retrospetiva com todos os campos através de um botão em Javascript</t>
   </si>
   <si>
     <t>Persistência - Frontend</t>
@@ -133,13 +130,31 @@
     <t>Opção de Alterar Língua (Inglês, Português)</t>
   </si>
   <si>
+    <t>S/T</t>
+  </si>
+  <si>
     <t>Stuff 2</t>
   </si>
   <si>
     <t>Opção de Alterar Cores (Dark, Light)</t>
   </si>
   <si>
-    <t/>
+    <t>Stuff 3</t>
+  </si>
+  <si>
+    <t>Opção no Settings para eliminar Utilizador(e toda a informação associada)</t>
+  </si>
+  <si>
+    <t>Stuff 4</t>
+  </si>
+  <si>
+    <t>Contador de Total de tarefas por cada board (To do - Doing - Done)</t>
+  </si>
+  <si>
+    <t>Stuff 5</t>
+  </si>
+  <si>
+    <t>Barra de progresso do Sprint com proporções que reflectem os valores do contador</t>
   </si>
 </sst>
 </file>
@@ -256,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -290,9 +305,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -619,13 +631,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="22.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="116.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="41.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="10.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="22.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="116.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="41.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -776,37 +788,37 @@
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -828,10 +840,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>9</v>
@@ -847,10 +859,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>9</v>
@@ -863,13 +875,13 @@
         <v>3</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>9</v>
@@ -885,10 +897,10 @@
         <v>13</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>9</v>
@@ -904,10 +916,10 @@
         <v>13</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>9</v>
@@ -920,16 +932,16 @@
         <v>6</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
@@ -951,10 +963,10 @@
         <v>6</v>
       </c>
       <c r="E20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>9</v>
@@ -970,10 +982,10 @@
         <v>13</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>9</v>
@@ -998,10 +1010,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>9</v>
@@ -1017,10 +1029,10 @@
         <v>13</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>9</v>
@@ -1039,14 +1051,16 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="G26" s="11"/>
     </row>
@@ -1054,7 +1068,9 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="E27" s="11" t="s">
         <v>39</v>
       </c>
@@ -1067,12 +1083,14 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="12" t="s">
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>41</v>
+      <c r="F28" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1080,18 +1098,30 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G30" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">

</xml_diff>